<commit_message>
Submitted report for Laboratory Class Equivalent Simulation
</commit_message>
<xml_diff>
--- a/Laboratory Class Equivalent Simulation/Part 1/Part-d.xlsx
+++ b/Laboratory Class Equivalent Simulation/Part 1/Part-d.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Power-Amplifier\Laboratory Class Equivalent Simulation\Part 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DE04EF-F058-4B4F-906A-005C31760075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0669F614-1391-488D-B830-7A832E1F8173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CBFA556-0710-4ABC-BEC4-A6B4AFBC3449}"/>
   </bookViews>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF142B0A-6EEB-4623-9088-39F8CA416835}">
   <dimension ref="A1:M329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N329" sqref="N329"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>